<commit_message>
Small Changes + New Hand Creator Function
Minor changes to Deck Creator function, plus a new Hand Creator Function which assigns 7 random cards to each player.
</commit_message>
<xml_diff>
--- a/ENG 006/Final Project/UNOCardTable.xlsx
+++ b/ENG 006/Final Project/UNOCardTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuval\Documents\MATLAB\ENG 006\Final Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ENG-006-Final-Project\ENG 006\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633C357B-3C5B-47AD-AA05-8C990D42AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C4720-D94F-4FDC-A4D3-39BAD2CB8C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15280" xr2:uid="{DD810E4E-5595-4EA2-BB40-9C3631E115DC}"/>
+    <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{DD810E4E-5595-4EA2-BB40-9C3631E115DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="65">
   <si>
     <t>UNO Cards</t>
   </si>
@@ -206,9 +206,6 @@
     <t>GreenDraw2</t>
   </si>
   <si>
-    <t>GreebDraw2</t>
-  </si>
-  <si>
     <t>YellowDraw2</t>
   </si>
   <si>
@@ -219,6 +216,21 @@
   </si>
   <si>
     <t>Played</t>
+  </si>
+  <si>
+    <t>Red0</t>
+  </si>
+  <si>
+    <t>Green0</t>
+  </si>
+  <si>
+    <t>Blue0</t>
+  </si>
+  <si>
+    <t>Yellow0</t>
+  </si>
+  <si>
+    <t>BlueDraw2</t>
   </si>
 </sst>
 </file>
@@ -569,7 +581,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -577,25 +589,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50A2126-E856-4693-A4C9-721E62201C74}">
-  <dimension ref="A1:E52"/>
+  <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.90625" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -607,392 +619,392 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
       <c r="D6">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E10" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>10</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E14" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E15" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>16</v>
+      <c r="B16" t="s">
+        <v>11</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E16" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>18</v>
+      <c r="B18" t="s">
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D18">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E18" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
+      <c r="B20" t="s">
+        <v>13</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D20">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E20" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D21">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E21" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>22</v>
+      <c r="B22" t="s">
+        <v>48</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D22">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E22" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D23">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E23" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D24">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D25">
         <v>11</v>
@@ -1001,15 +1013,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D26">
         <v>12</v>
@@ -1018,372 +1030,372 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="C27" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E27" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>61</v>
       </c>
       <c r="C28" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E28" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C29" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D29">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E29" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C30" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D30">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>29</v>
+      <c r="B31" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C31" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E31" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>30</v>
+      <c r="B32" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D32">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D33">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D34">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>33</v>
+      <c r="B35" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C35" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D35">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>50</v>
+      <c r="B36" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E36" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="C37" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D37">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="E37" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
       <c r="D38">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E38" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>34</v>
+      <c r="B39" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E39" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>35</v>
+      <c r="B40" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="C40" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D40">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="E40" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>21</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D41">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="C42" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>39</v>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D43">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>40</v>
+      <c r="B44" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D44">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E44" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="C45" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D45">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="C46" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C47" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D47">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E47" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C48" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D48">
         <v>10</v>
@@ -1392,15 +1404,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D49">
         <v>11</v>
@@ -1409,59 +1421,1049 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="D50">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E50" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="D51">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E51" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>50</v>
       </c>
       <c r="B52" t="s">
+        <v>55</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52">
+        <v>12</v>
+      </c>
+      <c r="E52" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>62</v>
+      </c>
+      <c r="C53" t="s">
+        <v>26</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>24</v>
+      </c>
+      <c r="C54" t="s">
+        <v>26</v>
+      </c>
+      <c r="D54">
+        <v>1</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>24</v>
+      </c>
+      <c r="C55" t="s">
+        <v>26</v>
+      </c>
+      <c r="D55">
+        <v>1</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C56" t="s">
+        <v>26</v>
+      </c>
+      <c r="D56">
+        <v>2</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>25</v>
+      </c>
+      <c r="C57" t="s">
+        <v>26</v>
+      </c>
+      <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58">
+        <v>3</v>
+      </c>
+      <c r="E58" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" t="s">
+        <v>26</v>
+      </c>
+      <c r="D59">
+        <v>3</v>
+      </c>
+      <c r="E59" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>58</v>
       </c>
-      <c r="C52" t="s">
+      <c r="B60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C60" t="s">
+        <v>26</v>
+      </c>
+      <c r="D60">
+        <v>4</v>
+      </c>
+      <c r="E60" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61" t="s">
+        <v>26</v>
+      </c>
+      <c r="D61">
+        <v>4</v>
+      </c>
+      <c r="E61" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>29</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62">
+        <v>5</v>
+      </c>
+      <c r="E62" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C63" t="s">
+        <v>26</v>
+      </c>
+      <c r="D63">
+        <v>5</v>
+      </c>
+      <c r="E63" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>30</v>
+      </c>
+      <c r="C64" t="s">
+        <v>26</v>
+      </c>
+      <c r="D64">
+        <v>6</v>
+      </c>
+      <c r="E64" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>30</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65">
+        <v>6</v>
+      </c>
+      <c r="E65" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C66" t="s">
+        <v>26</v>
+      </c>
+      <c r="D66">
+        <v>7</v>
+      </c>
+      <c r="E66" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>31</v>
+      </c>
+      <c r="C67" t="s">
+        <v>26</v>
+      </c>
+      <c r="D67">
+        <v>7</v>
+      </c>
+      <c r="E67" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>32</v>
+      </c>
+      <c r="C68" t="s">
+        <v>26</v>
+      </c>
+      <c r="D68">
+        <v>8</v>
+      </c>
+      <c r="E68" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>32</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69">
+        <v>8</v>
+      </c>
+      <c r="E69" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>33</v>
+      </c>
+      <c r="C70" t="s">
+        <v>26</v>
+      </c>
+      <c r="D70">
+        <v>9</v>
+      </c>
+      <c r="E70" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>33</v>
+      </c>
+      <c r="C71" t="s">
+        <v>26</v>
+      </c>
+      <c r="D71">
+        <v>9</v>
+      </c>
+      <c r="E71" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" t="s">
+        <v>26</v>
+      </c>
+      <c r="D72">
+        <v>10</v>
+      </c>
+      <c r="E72" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>50</v>
+      </c>
+      <c r="C73" t="s">
+        <v>26</v>
+      </c>
+      <c r="D73">
+        <v>10</v>
+      </c>
+      <c r="E73" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>46</v>
+      </c>
+      <c r="C74" t="s">
+        <v>26</v>
+      </c>
+      <c r="D74">
+        <v>11</v>
+      </c>
+      <c r="E74" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>46</v>
+      </c>
+      <c r="C75" t="s">
+        <v>26</v>
+      </c>
+      <c r="D75">
+        <v>11</v>
+      </c>
+      <c r="E75" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>64</v>
+      </c>
+      <c r="C76" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76">
+        <v>12</v>
+      </c>
+      <c r="E76" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>64</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+      <c r="D77">
+        <v>12</v>
+      </c>
+      <c r="E77" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>63</v>
+      </c>
+      <c r="C78" t="s">
+        <v>36</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" t="s">
+        <v>36</v>
+      </c>
+      <c r="D79">
+        <v>1</v>
+      </c>
+      <c r="E79" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" t="s">
+        <v>36</v>
+      </c>
+      <c r="D80">
+        <v>1</v>
+      </c>
+      <c r="E80" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>35</v>
+      </c>
+      <c r="C81" t="s">
+        <v>36</v>
+      </c>
+      <c r="D81">
+        <v>2</v>
+      </c>
+      <c r="E81" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>35</v>
+      </c>
+      <c r="C82" t="s">
+        <v>36</v>
+      </c>
+      <c r="D82">
+        <v>2</v>
+      </c>
+      <c r="E82" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>37</v>
+      </c>
+      <c r="C83" t="s">
+        <v>36</v>
+      </c>
+      <c r="D83">
+        <v>3</v>
+      </c>
+      <c r="E83" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>37</v>
+      </c>
+      <c r="C84" t="s">
+        <v>36</v>
+      </c>
+      <c r="D84">
+        <v>3</v>
+      </c>
+      <c r="E84" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>38</v>
+      </c>
+      <c r="C85" t="s">
+        <v>36</v>
+      </c>
+      <c r="D85">
+        <v>4</v>
+      </c>
+      <c r="E85" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86" t="s">
+        <v>38</v>
+      </c>
+      <c r="C86" t="s">
+        <v>36</v>
+      </c>
+      <c r="D86">
+        <v>4</v>
+      </c>
+      <c r="E86" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" t="s">
+        <v>36</v>
+      </c>
+      <c r="D87">
+        <v>5</v>
+      </c>
+      <c r="E87" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88" t="s">
+        <v>39</v>
+      </c>
+      <c r="C88" t="s">
+        <v>36</v>
+      </c>
+      <c r="D88">
+        <v>5</v>
+      </c>
+      <c r="E88" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89" t="s">
+        <v>40</v>
+      </c>
+      <c r="C89" t="s">
+        <v>36</v>
+      </c>
+      <c r="D89">
+        <v>6</v>
+      </c>
+      <c r="E89" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90" t="s">
+        <v>40</v>
+      </c>
+      <c r="C90" t="s">
+        <v>36</v>
+      </c>
+      <c r="D90">
+        <v>6</v>
+      </c>
+      <c r="E90" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91" t="s">
+        <v>41</v>
+      </c>
+      <c r="C91" t="s">
+        <v>36</v>
+      </c>
+      <c r="D91">
+        <v>7</v>
+      </c>
+      <c r="E91" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92" t="s">
+        <v>41</v>
+      </c>
+      <c r="C92" t="s">
+        <v>36</v>
+      </c>
+      <c r="D92">
+        <v>7</v>
+      </c>
+      <c r="E92" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93" t="s">
+        <v>42</v>
+      </c>
+      <c r="C93" t="s">
+        <v>36</v>
+      </c>
+      <c r="D93">
+        <v>8</v>
+      </c>
+      <c r="E93" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94" t="s">
+        <v>42</v>
+      </c>
+      <c r="C94" t="s">
+        <v>36</v>
+      </c>
+      <c r="D94">
+        <v>8</v>
+      </c>
+      <c r="E94" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95" t="s">
+        <v>43</v>
+      </c>
+      <c r="C95" t="s">
+        <v>36</v>
+      </c>
+      <c r="D95">
+        <v>9</v>
+      </c>
+      <c r="E95" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96" t="s">
+        <v>43</v>
+      </c>
+      <c r="C96" t="s">
+        <v>36</v>
+      </c>
+      <c r="D96">
+        <v>9</v>
+      </c>
+      <c r="E96" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97" t="s">
+        <v>51</v>
+      </c>
+      <c r="C97" t="s">
+        <v>36</v>
+      </c>
+      <c r="D97">
+        <v>10</v>
+      </c>
+      <c r="E97" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98" t="s">
+        <v>51</v>
+      </c>
+      <c r="C98" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98">
+        <v>10</v>
+      </c>
+      <c r="E98" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99" t="s">
+        <v>47</v>
+      </c>
+      <c r="C99" t="s">
+        <v>36</v>
+      </c>
+      <c r="D99">
+        <v>11</v>
+      </c>
+      <c r="E99" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100" t="s">
+        <v>47</v>
+      </c>
+      <c r="C100" t="s">
+        <v>36</v>
+      </c>
+      <c r="D100">
+        <v>11</v>
+      </c>
+      <c r="E100" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101" t="s">
+        <v>56</v>
+      </c>
+      <c r="C101" t="s">
+        <v>36</v>
+      </c>
+      <c r="D101">
+        <v>12</v>
+      </c>
+      <c r="E101" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102" t="s">
+        <v>56</v>
+      </c>
+      <c r="C102" t="s">
+        <v>36</v>
+      </c>
+      <c r="D102">
+        <v>12</v>
+      </c>
+      <c r="E102" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" t="s">
         <v>53</v>
       </c>
-      <c r="D52">
+      <c r="D103">
+        <v>13</v>
+      </c>
+      <c r="E103" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104" t="s">
+        <v>52</v>
+      </c>
+      <c r="C104" t="s">
+        <v>53</v>
+      </c>
+      <c r="D104">
+        <v>13</v>
+      </c>
+      <c r="E104" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105" t="s">
+        <v>52</v>
+      </c>
+      <c r="C105" t="s">
+        <v>53</v>
+      </c>
+      <c r="D105">
+        <v>13</v>
+      </c>
+      <c r="E105" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106" t="s">
+        <v>52</v>
+      </c>
+      <c r="C106" t="s">
+        <v>53</v>
+      </c>
+      <c r="D106">
+        <v>13</v>
+      </c>
+      <c r="E106" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <v>105</v>
+      </c>
+      <c r="B107" t="s">
+        <v>57</v>
+      </c>
+      <c r="C107" t="s">
+        <v>53</v>
+      </c>
+      <c r="D107">
         <v>14</v>
       </c>
-      <c r="E52" t="b">
+      <c r="E107" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <v>106</v>
+      </c>
+      <c r="B108" t="s">
+        <v>57</v>
+      </c>
+      <c r="C108" t="s">
+        <v>53</v>
+      </c>
+      <c r="D108">
+        <v>14</v>
+      </c>
+      <c r="E108" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <v>107</v>
+      </c>
+      <c r="B109" t="s">
+        <v>57</v>
+      </c>
+      <c r="C109" t="s">
+        <v>53</v>
+      </c>
+      <c r="D109">
+        <v>14</v>
+      </c>
+      <c r="E109" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <v>108</v>
+      </c>
+      <c r="B110" t="s">
+        <v>57</v>
+      </c>
+      <c r="C110" t="s">
+        <v>53</v>
+      </c>
+      <c r="D110">
+        <v>14</v>
+      </c>
+      <c r="E110" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E106">
+    <sortCondition ref="A4:A106"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Draw_Card, Place_Card, Minor Changes
Created 2 New Functions:

Draw_Card: Draws the card with the highest index with a Played value of false from UNOCardTable, switching that Played value to true, and adding that card to the hand of currentPlayer.

Place_Card: Obtains index of the previous card and selected card given their ID's, then checks if selected card can be placed. If the card can be placed, the card ID is replaced with a 0 in the player's hand, and the Played value of the selected card in UNOCardTable is switched back to false.

Minor Changes: fixed bug where Deck_Creator did not randomize every row, added semicolons in some other places.

I plan to continue working on Place_Card, potenitally adding functionality for checking the type of card and dealing with the consequences (wild, draw2, reverse, skip, etc.)
</commit_message>
<xml_diff>
--- a/ENG 006/Final Project/UNOCardTable.xlsx
+++ b/ENG 006/Final Project/UNOCardTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\ENG-006-Final-Project\ENG 006\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E5C4720-D94F-4FDC-A4D3-39BAD2CB8C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE91D1C7-2A40-4BF5-AD80-C2DDCAA28285}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="732" yWindow="732" windowWidth="17280" windowHeight="8880" xr2:uid="{DD810E4E-5595-4EA2-BB40-9C3631E115DC}"/>
   </bookViews>
@@ -173,9 +173,6 @@
     <t>RedReverse</t>
   </si>
   <si>
-    <t>GreedReverse</t>
-  </si>
-  <si>
     <t>BlueReverse</t>
   </si>
   <si>
@@ -231,6 +228,9 @@
   </si>
   <si>
     <t>BlueDraw2</t>
+  </si>
+  <si>
+    <t>GreenReverse</t>
   </si>
 </sst>
 </file>
@@ -591,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50A2126-E856-4693-A4C9-721E62201C74}">
   <dimension ref="A1:E110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -607,7 +607,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -619,7 +619,7 @@
         <v>3</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -627,7 +627,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -950,7 +950,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -967,7 +967,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -1018,7 +1018,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1035,7 +1035,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1052,7 +1052,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" t="s">
         <v>15</v>
@@ -1375,7 +1375,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
         <v>15</v>
@@ -1392,7 +1392,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C48" t="s">
         <v>15</v>
@@ -1409,7 +1409,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
         <v>15</v>
@@ -1426,7 +1426,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C50" t="s">
         <v>15</v>
@@ -1443,7 +1443,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C51" t="s">
         <v>15</v>
@@ -1460,7 +1460,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C52" t="s">
         <v>15</v>
@@ -1477,7 +1477,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" t="s">
         <v>26</v>
@@ -1800,7 +1800,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C72" t="s">
         <v>26</v>
@@ -1817,7 +1817,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C73" t="s">
         <v>26</v>
@@ -1834,7 +1834,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C74" t="s">
         <v>26</v>
@@ -1851,7 +1851,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C75" t="s">
         <v>26</v>
@@ -1868,7 +1868,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C76" t="s">
         <v>26</v>
@@ -1885,7 +1885,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C77" t="s">
         <v>26</v>
@@ -1902,7 +1902,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C78" t="s">
         <v>36</v>
@@ -2225,7 +2225,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C97" t="s">
         <v>36</v>
@@ -2242,7 +2242,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C98" t="s">
         <v>36</v>
@@ -2259,7 +2259,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C99" t="s">
         <v>36</v>
@@ -2276,7 +2276,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C100" t="s">
         <v>36</v>
@@ -2293,7 +2293,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C101" t="s">
         <v>36</v>
@@ -2310,7 +2310,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C102" t="s">
         <v>36</v>
@@ -2327,10 +2327,10 @@
         <v>101</v>
       </c>
       <c r="B103" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" t="s">
         <v>52</v>
-      </c>
-      <c r="C103" t="s">
-        <v>53</v>
       </c>
       <c r="D103">
         <v>13</v>
@@ -2344,10 +2344,10 @@
         <v>102</v>
       </c>
       <c r="B104" t="s">
+        <v>51</v>
+      </c>
+      <c r="C104" t="s">
         <v>52</v>
-      </c>
-      <c r="C104" t="s">
-        <v>53</v>
       </c>
       <c r="D104">
         <v>13</v>
@@ -2361,10 +2361,10 @@
         <v>103</v>
       </c>
       <c r="B105" t="s">
+        <v>51</v>
+      </c>
+      <c r="C105" t="s">
         <v>52</v>
-      </c>
-      <c r="C105" t="s">
-        <v>53</v>
       </c>
       <c r="D105">
         <v>13</v>
@@ -2378,10 +2378,10 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
+        <v>51</v>
+      </c>
+      <c r="C106" t="s">
         <v>52</v>
-      </c>
-      <c r="C106" t="s">
-        <v>53</v>
       </c>
       <c r="D106">
         <v>13</v>
@@ -2395,10 +2395,10 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C107" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D107">
         <v>14</v>
@@ -2412,10 +2412,10 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C108" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D108">
         <v>14</v>
@@ -2429,10 +2429,10 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C109" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D109">
         <v>14</v>
@@ -2446,10 +2446,10 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C110" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D110">
         <v>14</v>

</xml_diff>

<commit_message>
Random stuff that I screwed up/ Core Final Project
S
</commit_message>
<xml_diff>
--- a/ENG 006/Final Project/UNOCardTable.xlsx
+++ b/ENG 006/Final Project/UNOCardTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kuval\Documents\GitHub\ENG-006-Final-Project\ENG 006\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49044C5B-EE43-4722-AB71-46DD6BA5774E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C016AD2-0591-45FC-ABD3-E0807B9D559E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15280" xr2:uid="{DD810E4E-5595-4EA2-BB40-9C3631E115DC}"/>
   </bookViews>
@@ -71,166 +71,166 @@
     <t>Played</t>
   </si>
   <si>
-    <t>Red0.jpg</t>
-  </si>
-  <si>
-    <t>Red1.jpg</t>
-  </si>
-  <si>
-    <t>Red2.jpg</t>
-  </si>
-  <si>
-    <t>Red3.jpg</t>
-  </si>
-  <si>
-    <t>Red4.jpg</t>
-  </si>
-  <si>
-    <t>Red5.jpg</t>
-  </si>
-  <si>
-    <t>Red6.jpg</t>
-  </si>
-  <si>
-    <t>Red7.jpg</t>
-  </si>
-  <si>
-    <t>Red8.jpg</t>
-  </si>
-  <si>
-    <t>Red9.jpg</t>
-  </si>
-  <si>
-    <t>RedSkip.jpg</t>
-  </si>
-  <si>
-    <t>RedReverse.jpg</t>
-  </si>
-  <si>
-    <t>RedDraw2.jpg</t>
-  </si>
-  <si>
-    <t>Green0.jpg</t>
-  </si>
-  <si>
-    <t>Green1.jpg</t>
-  </si>
-  <si>
-    <t>Green2.jpg</t>
-  </si>
-  <si>
-    <t>Green3.jpg</t>
-  </si>
-  <si>
-    <t>Green4.jpg</t>
-  </si>
-  <si>
-    <t>Green5.jpg</t>
-  </si>
-  <si>
-    <t>Green6.jpg</t>
-  </si>
-  <si>
-    <t>Green7.jpg</t>
-  </si>
-  <si>
-    <t>Green8.jpg</t>
-  </si>
-  <si>
-    <t>Green9.jpg</t>
-  </si>
-  <si>
-    <t>GreenSkip.jpg</t>
-  </si>
-  <si>
-    <t>GreenReverse.jpg</t>
-  </si>
-  <si>
-    <t>GreenDraw2.jpg</t>
-  </si>
-  <si>
-    <t>Blue0.jpg</t>
-  </si>
-  <si>
-    <t>Blue1.jpg</t>
-  </si>
-  <si>
-    <t>Blue2.jpg</t>
-  </si>
-  <si>
-    <t>Blue3.jpg</t>
-  </si>
-  <si>
-    <t>Blue4.jpg</t>
-  </si>
-  <si>
-    <t>Blue5.jpg</t>
-  </si>
-  <si>
-    <t>Blue6.jpg</t>
-  </si>
-  <si>
-    <t>Blue7.jpg</t>
-  </si>
-  <si>
-    <t>Blue8.jpg</t>
-  </si>
-  <si>
-    <t>Blue9.jpg</t>
-  </si>
-  <si>
-    <t>BlueSkip.jpg</t>
-  </si>
-  <si>
-    <t>BlueReverse.jpg</t>
-  </si>
-  <si>
-    <t>BlueDraw2.jpg</t>
-  </si>
-  <si>
-    <t>Yellow0.jpg</t>
-  </si>
-  <si>
-    <t>Yellow1.jpg</t>
-  </si>
-  <si>
-    <t>Yellow2.jpg</t>
-  </si>
-  <si>
-    <t>Yellow3.jpg</t>
-  </si>
-  <si>
-    <t>Yellow4.jpg</t>
-  </si>
-  <si>
-    <t>Yellow5.jpg</t>
-  </si>
-  <si>
-    <t>Yellow6.jpg</t>
-  </si>
-  <si>
-    <t>Yellow7.jpg</t>
-  </si>
-  <si>
-    <t>Yellow8.jpg</t>
-  </si>
-  <si>
-    <t>Yellow9.jpg</t>
-  </si>
-  <si>
-    <t>YellowSkip.jpg</t>
-  </si>
-  <si>
-    <t>YellowReverse.jpg</t>
-  </si>
-  <si>
-    <t>YellowDraw2.jpg</t>
-  </si>
-  <si>
-    <t>WildCard.jpg</t>
-  </si>
-  <si>
-    <t>Draw4.jpg</t>
+    <t>Red0</t>
+  </si>
+  <si>
+    <t>Red1</t>
+  </si>
+  <si>
+    <t>Red2</t>
+  </si>
+  <si>
+    <t>Red3</t>
+  </si>
+  <si>
+    <t>Red4</t>
+  </si>
+  <si>
+    <t>Red5</t>
+  </si>
+  <si>
+    <t>Red6</t>
+  </si>
+  <si>
+    <t>Red7</t>
+  </si>
+  <si>
+    <t>Red8</t>
+  </si>
+  <si>
+    <t>Red9</t>
+  </si>
+  <si>
+    <t>Green0</t>
+  </si>
+  <si>
+    <t>Green1</t>
+  </si>
+  <si>
+    <t>Green2</t>
+  </si>
+  <si>
+    <t>Green3</t>
+  </si>
+  <si>
+    <t>Green4</t>
+  </si>
+  <si>
+    <t>Green5</t>
+  </si>
+  <si>
+    <t>Green6</t>
+  </si>
+  <si>
+    <t>Green7</t>
+  </si>
+  <si>
+    <t>Green8</t>
+  </si>
+  <si>
+    <t>Green9</t>
+  </si>
+  <si>
+    <t>Blue0</t>
+  </si>
+  <si>
+    <t>Blue1</t>
+  </si>
+  <si>
+    <t>Blue2</t>
+  </si>
+  <si>
+    <t>Blue3</t>
+  </si>
+  <si>
+    <t>Blue4</t>
+  </si>
+  <si>
+    <t>Blue5</t>
+  </si>
+  <si>
+    <t>Blue6</t>
+  </si>
+  <si>
+    <t>Blue7</t>
+  </si>
+  <si>
+    <t>Blue8</t>
+  </si>
+  <si>
+    <t>Blue9</t>
+  </si>
+  <si>
+    <t>Yellow0</t>
+  </si>
+  <si>
+    <t>Yellow1</t>
+  </si>
+  <si>
+    <t>Yellow2</t>
+  </si>
+  <si>
+    <t>Yellow3</t>
+  </si>
+  <si>
+    <t>Yellow4</t>
+  </si>
+  <si>
+    <t>Yellow5</t>
+  </si>
+  <si>
+    <t>Yellow6</t>
+  </si>
+  <si>
+    <t>Yellow7</t>
+  </si>
+  <si>
+    <t>Yellow8</t>
+  </si>
+  <si>
+    <t>Yellow9</t>
+  </si>
+  <si>
+    <t>RedSkip</t>
+  </si>
+  <si>
+    <t>RedReverse</t>
+  </si>
+  <si>
+    <t>RedDraw2</t>
+  </si>
+  <si>
+    <t>GreenSkip</t>
+  </si>
+  <si>
+    <t>GreenReverse</t>
+  </si>
+  <si>
+    <t>GreenDraw2</t>
+  </si>
+  <si>
+    <t>BlueSkip</t>
+  </si>
+  <si>
+    <t>BlueReverse</t>
+  </si>
+  <si>
+    <t>BlueDraw2</t>
+  </si>
+  <si>
+    <t>YellowSkip</t>
+  </si>
+  <si>
+    <t>YellowReverse</t>
+  </si>
+  <si>
+    <t>YellowDraw2</t>
+  </si>
+  <si>
+    <t>WildCard</t>
+  </si>
+  <si>
+    <t>Draw4</t>
   </si>
 </sst>
 </file>
@@ -272,9 +272,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -589,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C50A2126-E856-4693-A4C9-721E62201C74}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B75" workbookViewId="0">
+      <selection activeCell="O94" sqref="O94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -600,12 +599,12 @@
     <col min="2" max="2" width="13.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -621,13 +620,17 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
+      <c r="B3" t="str">
+        <f>_xlfn.CONCAT(K2 &amp; ".png")</f>
+        <v>Red0.png</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -638,13 +641,17 @@
       <c r="E3" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4" t="str">
+        <f t="shared" ref="B4:B67" si="0">_xlfn.CONCAT(K3 &amp; ".png")</f>
+        <v>Red1.png</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
@@ -655,13 +662,17 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
+      <c r="B5" t="str">
+        <f t="shared" si="0"/>
+        <v>Red1.png</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -672,13 +683,17 @@
       <c r="E5" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>13</v>
+      <c r="B6" t="str">
+        <f t="shared" si="0"/>
+        <v>Red2.png</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -689,13 +704,17 @@
       <c r="E6" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>13</v>
+      <c r="B7" t="str">
+        <f t="shared" si="0"/>
+        <v>Red2.png</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -706,13 +725,17 @@
       <c r="E7" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>14</v>
+      <c r="B8" t="str">
+        <f t="shared" si="0"/>
+        <v>Red3.png</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -723,13 +746,17 @@
       <c r="E8" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>14</v>
+      <c r="B9" t="str">
+        <f t="shared" si="0"/>
+        <v>Red3.png</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
@@ -740,30 +767,38 @@
       <c r="E9" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="str">
+        <f t="shared" si="0"/>
+        <v>Red4.png</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="s">
         <v>15</v>
       </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
+      <c r="B11" t="str">
+        <f t="shared" si="0"/>
+        <v>Red4.png</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -774,30 +809,38 @@
       <c r="E11" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="str">
+        <f t="shared" si="0"/>
+        <v>Red5.png</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="s">
         <v>16</v>
       </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>16</v>
+      <c r="B13" t="str">
+        <f t="shared" si="0"/>
+        <v>Red5.png</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -808,30 +851,38 @@
       <c r="E13" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="str">
+        <f t="shared" si="0"/>
+        <v>Red6.png</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="s">
         <v>17</v>
       </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14">
-        <v>6</v>
-      </c>
-      <c r="E14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>17</v>
+      <c r="B15" t="str">
+        <f t="shared" si="0"/>
+        <v>Red6.png</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
@@ -842,30 +893,38 @@
       <c r="E15" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="str">
+        <f t="shared" si="0"/>
+        <v>Red7.png</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-      <c r="E16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>18</v>
+      <c r="B17" t="str">
+        <f t="shared" si="0"/>
+        <v>Red7.png</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
@@ -876,13 +935,17 @@
       <c r="E17" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>19</v>
+      <c r="B18" t="str">
+        <f t="shared" si="0"/>
+        <v>Red8.png</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -893,13 +956,17 @@
       <c r="E18" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>19</v>
+      <c r="B19" t="str">
+        <f t="shared" si="0"/>
+        <v>Red8.png</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -910,13 +977,17 @@
       <c r="E19" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>20</v>
+      <c r="B20" t="str">
+        <f t="shared" si="0"/>
+        <v>Red9.png</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
@@ -927,13 +998,17 @@
       <c r="E20" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
+      <c r="B21" t="str">
+        <f t="shared" si="0"/>
+        <v>Red9.png</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
@@ -944,13 +1019,17 @@
       <c r="E21" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K21" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>21</v>
+      <c r="B22" t="str">
+        <f t="shared" si="0"/>
+        <v>RedSkip.png</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
@@ -961,13 +1040,17 @@
       <c r="E22" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>21</v>
+      <c r="B23" t="str">
+        <f t="shared" si="0"/>
+        <v>RedSkip.png</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -978,13 +1061,17 @@
       <c r="E23" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>22</v>
+      <c r="B24" t="str">
+        <f t="shared" si="0"/>
+        <v>RedReverse.png</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -995,13 +1082,17 @@
       <c r="E24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>22</v>
+      <c r="B25" t="str">
+        <f t="shared" si="0"/>
+        <v>RedReverse.png</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -1012,13 +1103,17 @@
       <c r="E25" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K25" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>23</v>
+      <c r="B26" t="str">
+        <f t="shared" si="0"/>
+        <v>RedDraw2.png</v>
       </c>
       <c r="C26" t="s">
         <v>4</v>
@@ -1029,13 +1124,17 @@
       <c r="E26" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>23</v>
+      <c r="B27" t="str">
+        <f t="shared" si="0"/>
+        <v>RedDraw2.png</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -1046,13 +1145,17 @@
       <c r="E27" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>24</v>
+      <c r="B28" t="str">
+        <f t="shared" si="0"/>
+        <v>Green0.png</v>
       </c>
       <c r="C28" t="s">
         <v>5</v>
@@ -1063,13 +1166,17 @@
       <c r="E28" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>25</v>
+      <c r="B29" t="str">
+        <f t="shared" si="0"/>
+        <v>Green1.png</v>
       </c>
       <c r="C29" t="s">
         <v>5</v>
@@ -1080,13 +1187,17 @@
       <c r="E29" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>25</v>
+      <c r="B30" t="str">
+        <f t="shared" si="0"/>
+        <v>Green1.png</v>
       </c>
       <c r="C30" t="s">
         <v>5</v>
@@ -1097,13 +1208,17 @@
       <c r="E30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K30" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>26</v>
+      <c r="B31" t="str">
+        <f t="shared" si="0"/>
+        <v>Green2.png</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -1114,13 +1229,17 @@
       <c r="E31" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>26</v>
+      <c r="B32" t="str">
+        <f t="shared" si="0"/>
+        <v>Green2.png</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -1131,13 +1250,17 @@
       <c r="E32" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>27</v>
+      <c r="B33" t="str">
+        <f t="shared" si="0"/>
+        <v>Green3.png</v>
       </c>
       <c r="C33" t="s">
         <v>5</v>
@@ -1148,13 +1271,17 @@
       <c r="E33" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>27</v>
+      <c r="B34" t="str">
+        <f t="shared" si="0"/>
+        <v>Green3.png</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
@@ -1165,13 +1292,17 @@
       <c r="E34" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>28</v>
+      <c r="B35" t="str">
+        <f t="shared" si="0"/>
+        <v>Green4.png</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -1182,13 +1313,17 @@
       <c r="E35" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>28</v>
+      <c r="B36" t="str">
+        <f t="shared" si="0"/>
+        <v>Green4.png</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
@@ -1199,13 +1334,17 @@
       <c r="E36" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K36" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>29</v>
+      <c r="B37" t="str">
+        <f t="shared" si="0"/>
+        <v>Green5.png</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
@@ -1216,13 +1355,17 @@
       <c r="E37" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K37" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
-        <v>29</v>
+      <c r="B38" t="str">
+        <f t="shared" si="0"/>
+        <v>Green5.png</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
@@ -1233,13 +1376,17 @@
       <c r="E38" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K38" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>30</v>
+      <c r="B39" t="str">
+        <f t="shared" si="0"/>
+        <v>Green6.png</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
@@ -1250,13 +1397,17 @@
       <c r="E39" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K39" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>30</v>
+      <c r="B40" t="str">
+        <f t="shared" si="0"/>
+        <v>Green6.png</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
@@ -1267,13 +1418,17 @@
       <c r="E40" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K40" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>31</v>
+      <c r="B41" t="str">
+        <f t="shared" si="0"/>
+        <v>Green7.png</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
@@ -1284,13 +1439,17 @@
       <c r="E41" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K41" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>31</v>
+      <c r="B42" t="str">
+        <f t="shared" si="0"/>
+        <v>Green7.png</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -1301,13 +1460,17 @@
       <c r="E42" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K42" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>32</v>
+      <c r="B43" t="str">
+        <f t="shared" si="0"/>
+        <v>Green8.png</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -1318,13 +1481,17 @@
       <c r="E43" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K43" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>32</v>
+      <c r="B44" t="str">
+        <f t="shared" si="0"/>
+        <v>Green8.png</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
@@ -1335,13 +1502,17 @@
       <c r="E44" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K44" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
-        <v>33</v>
+      <c r="B45" t="str">
+        <f t="shared" si="0"/>
+        <v>Green9.png</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -1352,13 +1523,17 @@
       <c r="E45" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K45" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
-        <v>33</v>
+      <c r="B46" t="str">
+        <f t="shared" si="0"/>
+        <v>Green9.png</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -1369,13 +1544,17 @@
       <c r="E46" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
-        <v>34</v>
+      <c r="B47" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenSkip.png</v>
       </c>
       <c r="C47" t="s">
         <v>5</v>
@@ -1386,13 +1565,17 @@
       <c r="E47" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>34</v>
+      <c r="B48" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenSkip.png</v>
       </c>
       <c r="C48" t="s">
         <v>5</v>
@@ -1403,13 +1586,17 @@
       <c r="E48" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K48" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
-        <v>35</v>
+      <c r="B49" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenReverse.png</v>
       </c>
       <c r="C49" t="s">
         <v>5</v>
@@ -1420,13 +1607,17 @@
       <c r="E49" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K49" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
-        <v>35</v>
+      <c r="B50" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenReverse.png</v>
       </c>
       <c r="C50" t="s">
         <v>5</v>
@@ -1437,13 +1628,17 @@
       <c r="E50" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
-        <v>36</v>
+      <c r="B51" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenDraw2.png</v>
       </c>
       <c r="C51" t="s">
         <v>5</v>
@@ -1454,13 +1649,17 @@
       <c r="E51" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>36</v>
+      <c r="B52" t="str">
+        <f t="shared" si="0"/>
+        <v>GreenDraw2.png</v>
       </c>
       <c r="C52" t="s">
         <v>5</v>
@@ -1471,13 +1670,17 @@
       <c r="E52" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K52" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
-        <v>37</v>
+      <c r="B53" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue0.png</v>
       </c>
       <c r="C53" t="s">
         <v>6</v>
@@ -1488,13 +1691,17 @@
       <c r="E53" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K53" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
-        <v>38</v>
+      <c r="B54" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue1.png</v>
       </c>
       <c r="C54" t="s">
         <v>6</v>
@@ -1505,13 +1712,17 @@
       <c r="E54" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K54" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
-        <v>38</v>
+      <c r="B55" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue1.png</v>
       </c>
       <c r="C55" t="s">
         <v>6</v>
@@ -1522,13 +1733,17 @@
       <c r="E55" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K55" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
-        <v>39</v>
+      <c r="B56" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue2.png</v>
       </c>
       <c r="C56" t="s">
         <v>6</v>
@@ -1539,13 +1754,17 @@
       <c r="E56" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K56" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
-        <v>39</v>
+      <c r="B57" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue2.png</v>
       </c>
       <c r="C57" t="s">
         <v>6</v>
@@ -1556,13 +1775,17 @@
       <c r="E57" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K57" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
-        <v>40</v>
+      <c r="B58" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue3.png</v>
       </c>
       <c r="C58" t="s">
         <v>6</v>
@@ -1573,13 +1796,17 @@
       <c r="E58" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K58" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
-        <v>40</v>
+      <c r="B59" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue3.png</v>
       </c>
       <c r="C59" t="s">
         <v>6</v>
@@ -1590,13 +1817,17 @@
       <c r="E59" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K59" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
-        <v>41</v>
+      <c r="B60" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue4.png</v>
       </c>
       <c r="C60" t="s">
         <v>6</v>
@@ -1607,13 +1838,17 @@
       <c r="E60" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K60" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
-        <v>41</v>
+      <c r="B61" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue4.png</v>
       </c>
       <c r="C61" t="s">
         <v>6</v>
@@ -1624,13 +1859,17 @@
       <c r="E61" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K61" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
-        <v>42</v>
+      <c r="B62" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue5.png</v>
       </c>
       <c r="C62" t="s">
         <v>6</v>
@@ -1641,13 +1880,17 @@
       <c r="E62" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K62" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>42</v>
+      <c r="B63" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue5.png</v>
       </c>
       <c r="C63" t="s">
         <v>6</v>
@@ -1658,13 +1901,17 @@
       <c r="E63" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K63" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
-        <v>43</v>
+      <c r="B64" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue6.png</v>
       </c>
       <c r="C64" t="s">
         <v>6</v>
@@ -1675,13 +1922,17 @@
       <c r="E64" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K64" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
-        <v>43</v>
+      <c r="B65" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue6.png</v>
       </c>
       <c r="C65" t="s">
         <v>6</v>
@@ -1692,13 +1943,17 @@
       <c r="E65" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K65" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
-        <v>44</v>
+      <c r="B66" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue7.png</v>
       </c>
       <c r="C66" t="s">
         <v>6</v>
@@ -1709,13 +1964,17 @@
       <c r="E66" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K66" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
-        <v>44</v>
+      <c r="B67" t="str">
+        <f t="shared" si="0"/>
+        <v>Blue7.png</v>
       </c>
       <c r="C67" t="s">
         <v>6</v>
@@ -1726,13 +1985,17 @@
       <c r="E67" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K67" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
-        <v>45</v>
+      <c r="B68" t="str">
+        <f t="shared" ref="B68:B110" si="1">_xlfn.CONCAT(K67 &amp; ".png")</f>
+        <v>Blue8.png</v>
       </c>
       <c r="C68" t="s">
         <v>6</v>
@@ -1743,13 +2006,17 @@
       <c r="E68" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
-        <v>45</v>
+      <c r="B69" t="str">
+        <f t="shared" si="1"/>
+        <v>Blue8.png</v>
       </c>
       <c r="C69" t="s">
         <v>6</v>
@@ -1760,13 +2027,17 @@
       <c r="E69" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K69" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="s">
-        <v>46</v>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>Blue9.png</v>
       </c>
       <c r="C70" t="s">
         <v>6</v>
@@ -1777,13 +2048,17 @@
       <c r="E70" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K70" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
-        <v>46</v>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>Blue9.png</v>
       </c>
       <c r="C71" t="s">
         <v>6</v>
@@ -1794,13 +2069,17 @@
       <c r="E71" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K71" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
-        <v>47</v>
+      <c r="B72" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueSkip.png</v>
       </c>
       <c r="C72" t="s">
         <v>6</v>
@@ -1811,13 +2090,17 @@
       <c r="E72" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K72" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
-        <v>47</v>
+      <c r="B73" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueSkip.png</v>
       </c>
       <c r="C73" t="s">
         <v>6</v>
@@ -1828,13 +2111,17 @@
       <c r="E73" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K73" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
-        <v>48</v>
+      <c r="B74" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueReverse.png</v>
       </c>
       <c r="C74" t="s">
         <v>6</v>
@@ -1845,13 +2132,17 @@
       <c r="E74" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K74" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" t="s">
-        <v>48</v>
+      <c r="B75" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueReverse.png</v>
       </c>
       <c r="C75" t="s">
         <v>6</v>
@@ -1862,13 +2153,17 @@
       <c r="E75" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K75" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" t="s">
-        <v>49</v>
+      <c r="B76" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueDraw2.png</v>
       </c>
       <c r="C76" t="s">
         <v>6</v>
@@ -1879,13 +2174,17 @@
       <c r="E76" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K76" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
-        <v>49</v>
+      <c r="B77" t="str">
+        <f t="shared" si="1"/>
+        <v>BlueDraw2.png</v>
       </c>
       <c r="C77" t="s">
         <v>6</v>
@@ -1896,13 +2195,17 @@
       <c r="E77" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K77" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" t="s">
-        <v>50</v>
+      <c r="B78" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow0.png</v>
       </c>
       <c r="C78" t="s">
         <v>7</v>
@@ -1913,13 +2216,17 @@
       <c r="E78" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K78" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" t="s">
-        <v>51</v>
+      <c r="B79" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow1.png</v>
       </c>
       <c r="C79" t="s">
         <v>7</v>
@@ -1930,13 +2237,17 @@
       <c r="E79" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K79" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
-        <v>51</v>
+      <c r="B80" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow1.png</v>
       </c>
       <c r="C80" t="s">
         <v>7</v>
@@ -1947,13 +2258,17 @@
       <c r="E80" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K80" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
-        <v>52</v>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow2.png</v>
       </c>
       <c r="C81" t="s">
         <v>7</v>
@@ -1964,13 +2279,17 @@
       <c r="E81" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K81" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
-        <v>52</v>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow2.png</v>
       </c>
       <c r="C82" t="s">
         <v>7</v>
@@ -1981,13 +2300,17 @@
       <c r="E82" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K82" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" t="s">
-        <v>53</v>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow3.png</v>
       </c>
       <c r="C83" t="s">
         <v>7</v>
@@ -1998,13 +2321,17 @@
       <c r="E83" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K83" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
-        <v>53</v>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow3.png</v>
       </c>
       <c r="C84" t="s">
         <v>7</v>
@@ -2015,13 +2342,17 @@
       <c r="E84" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K84" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
-        <v>54</v>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow4.png</v>
       </c>
       <c r="C85" t="s">
         <v>7</v>
@@ -2032,13 +2363,17 @@
       <c r="E85" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K85" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" t="s">
-        <v>54</v>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow4.png</v>
       </c>
       <c r="C86" t="s">
         <v>7</v>
@@ -2049,13 +2384,17 @@
       <c r="E86" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K86" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
-        <v>55</v>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow5.png</v>
       </c>
       <c r="C87" t="s">
         <v>7</v>
@@ -2066,13 +2405,17 @@
       <c r="E87" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K87" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" t="s">
-        <v>55</v>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow5.png</v>
       </c>
       <c r="C88" t="s">
         <v>7</v>
@@ -2083,13 +2426,17 @@
       <c r="E88" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K88" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" t="s">
-        <v>56</v>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow6.png</v>
       </c>
       <c r="C89" t="s">
         <v>7</v>
@@ -2100,13 +2447,17 @@
       <c r="E89" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" t="s">
-        <v>56</v>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow6.png</v>
       </c>
       <c r="C90" t="s">
         <v>7</v>
@@ -2117,13 +2468,17 @@
       <c r="E90" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K90" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" t="s">
-        <v>57</v>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow7.png</v>
       </c>
       <c r="C91" t="s">
         <v>7</v>
@@ -2134,13 +2489,17 @@
       <c r="E91" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K91" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" t="s">
-        <v>57</v>
+      <c r="B92" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow7.png</v>
       </c>
       <c r="C92" t="s">
         <v>7</v>
@@ -2151,13 +2510,17 @@
       <c r="E92" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K92" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" t="s">
-        <v>58</v>
+      <c r="B93" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow8.png</v>
       </c>
       <c r="C93" t="s">
         <v>7</v>
@@ -2168,13 +2531,17 @@
       <c r="E93" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K93" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
-        <v>58</v>
+      <c r="B94" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow8.png</v>
       </c>
       <c r="C94" t="s">
         <v>7</v>
@@ -2185,13 +2552,17 @@
       <c r="E94" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K94" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
-        <v>59</v>
+      <c r="B95" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow9.png</v>
       </c>
       <c r="C95" t="s">
         <v>7</v>
@@ -2202,13 +2573,17 @@
       <c r="E95" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K95" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
-        <v>59</v>
+      <c r="B96" t="str">
+        <f t="shared" si="1"/>
+        <v>Yellow9.png</v>
       </c>
       <c r="C96" t="s">
         <v>7</v>
@@ -2219,13 +2594,17 @@
       <c r="E96" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K96" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" t="s">
-        <v>60</v>
+      <c r="B97" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowSkip.png</v>
       </c>
       <c r="C97" t="s">
         <v>7</v>
@@ -2236,13 +2615,17 @@
       <c r="E97" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K97" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" t="s">
-        <v>60</v>
+      <c r="B98" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowSkip.png</v>
       </c>
       <c r="C98" t="s">
         <v>7</v>
@@ -2253,13 +2636,17 @@
       <c r="E98" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K98" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" t="s">
-        <v>61</v>
+      <c r="B99" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowReverse.png</v>
       </c>
       <c r="C99" t="s">
         <v>7</v>
@@ -2270,13 +2657,17 @@
       <c r="E99" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K99" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" t="s">
-        <v>61</v>
+      <c r="B100" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowReverse.png</v>
       </c>
       <c r="C100" t="s">
         <v>7</v>
@@ -2287,13 +2678,17 @@
       <c r="E100" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K100" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" t="s">
-        <v>62</v>
+      <c r="B101" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowDraw2.png</v>
       </c>
       <c r="C101" t="s">
         <v>7</v>
@@ -2304,13 +2699,17 @@
       <c r="E101" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K101" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>100</v>
       </c>
-      <c r="B102" t="s">
-        <v>62</v>
+      <c r="B102" t="str">
+        <f t="shared" si="1"/>
+        <v>YellowDraw2.png</v>
       </c>
       <c r="C102" t="s">
         <v>7</v>
@@ -2321,13 +2720,17 @@
       <c r="E102" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K102" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>101</v>
       </c>
-      <c r="B103" t="s">
-        <v>63</v>
+      <c r="B103" t="str">
+        <f t="shared" si="1"/>
+        <v>WildCard.png</v>
       </c>
       <c r="C103" t="s">
         <v>8</v>
@@ -2338,13 +2741,17 @@
       <c r="E103" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K103" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>102</v>
       </c>
-      <c r="B104" t="s">
-        <v>63</v>
+      <c r="B104" t="str">
+        <f t="shared" si="1"/>
+        <v>WildCard.png</v>
       </c>
       <c r="C104" t="s">
         <v>8</v>
@@ -2355,13 +2762,17 @@
       <c r="E104" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K104" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>103</v>
       </c>
-      <c r="B105" t="s">
-        <v>63</v>
+      <c r="B105" t="str">
+        <f t="shared" si="1"/>
+        <v>WildCard.png</v>
       </c>
       <c r="C105" t="s">
         <v>8</v>
@@ -2372,13 +2783,17 @@
       <c r="E105" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K105" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>104</v>
       </c>
-      <c r="B106" t="s">
-        <v>63</v>
+      <c r="B106" t="str">
+        <f t="shared" si="1"/>
+        <v>WildCard.png</v>
       </c>
       <c r="C106" t="s">
         <v>8</v>
@@ -2389,13 +2804,17 @@
       <c r="E106" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K106" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>105</v>
       </c>
-      <c r="B107" t="s">
-        <v>64</v>
+      <c r="B107" t="str">
+        <f t="shared" si="1"/>
+        <v>Draw4.png</v>
       </c>
       <c r="C107" t="s">
         <v>8</v>
@@ -2406,13 +2825,17 @@
       <c r="E107" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K107" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>106</v>
       </c>
-      <c r="B108" t="s">
-        <v>64</v>
+      <c r="B108" t="str">
+        <f t="shared" si="1"/>
+        <v>Draw4.png</v>
       </c>
       <c r="C108" t="s">
         <v>8</v>
@@ -2423,13 +2846,17 @@
       <c r="E108" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K108" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>107</v>
       </c>
-      <c r="B109" t="s">
-        <v>64</v>
+      <c r="B109" t="str">
+        <f t="shared" si="1"/>
+        <v>Draw4.png</v>
       </c>
       <c r="C109" t="s">
         <v>8</v>
@@ -2440,13 +2867,17 @@
       <c r="E109" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="K109" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>108</v>
       </c>
-      <c r="B110" t="s">
-        <v>64</v>
+      <c r="B110" t="str">
+        <f t="shared" si="1"/>
+        <v>Draw4.png</v>
       </c>
       <c r="C110" t="s">
         <v>8</v>

</xml_diff>